<commit_message>
Final Update for SMP Working Paper
</commit_message>
<xml_diff>
--- a/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/CAAggregated C-A  Diff-in-DiffDAGVAR 2010-01-31 to 2020-02-29.xlsx
+++ b/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/CAAggregated C-A  Diff-in-DiffDAGVAR 2010-01-31 to 2020-02-29.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>C/A</t>
   </si>
@@ -22,9 +22,6 @@
     <t>FFR</t>
   </si>
   <si>
-    <t>LF</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -34,34 +31,16 @@
     <t>FFR Lag</t>
   </si>
   <si>
-    <t>LF Lag</t>
-  </si>
-  <si>
-    <t>-0.699***</t>
-  </si>
-  <si>
-    <t>9.766***</t>
-  </si>
-  <si>
-    <t>0.041</t>
-  </si>
-  <si>
-    <t>-0.029***</t>
-  </si>
-  <si>
-    <t>0.395***</t>
-  </si>
-  <si>
-    <t>-0.006</t>
-  </si>
-  <si>
-    <t>-0.235***</t>
-  </si>
-  <si>
-    <t>10.288***</t>
-  </si>
-  <si>
-    <t>-0.136*</t>
+    <t>-0.68***</t>
+  </si>
+  <si>
+    <t>9.556***</t>
+  </si>
+  <si>
+    <t>-0.032***</t>
+  </si>
+  <si>
+    <t>0.426***</t>
   </si>
 </sst>
 </file>
@@ -419,15 +398,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -435,50 +414,27 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rebuild ADF test for annual rates and lags / monthly freq
</commit_message>
<xml_diff>
--- a/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/CAAggregated C-A  Diff-in-DiffDAGVAR 2010-01-31 to 2020-02-29.xlsx
+++ b/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/CAAggregated C-A  Diff-in-DiffDAGVAR 2010-01-31 to 2020-02-29.xlsx
@@ -19,7 +19,7 @@
     <t>C/A</t>
   </si>
   <si>
-    <t>FFR</t>
+    <t>LF</t>
   </si>
   <si>
     <t>Source</t>
@@ -28,19 +28,19 @@
     <t>C/A Lag</t>
   </si>
   <si>
-    <t>FFR Lag</t>
-  </si>
-  <si>
-    <t>-0.68***</t>
-  </si>
-  <si>
-    <t>9.556***</t>
-  </si>
-  <si>
-    <t>-0.032***</t>
-  </si>
-  <si>
-    <t>0.426***</t>
+    <t>LF Lag</t>
+  </si>
+  <si>
+    <t>-0.326***</t>
+  </si>
+  <si>
+    <t>-0.261*</t>
+  </si>
+  <si>
+    <t>0.159</t>
+  </si>
+  <si>
+    <t>-0.454**</t>
   </si>
 </sst>
 </file>

</xml_diff>